<commit_message>
- fix association rules with label
</commit_message>
<xml_diff>
--- a/DSBot/kb.xlsx
+++ b/DSBot/kb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarapido/Desktop/DSBot/DSBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1773FE5-303A-7C4B-A6A1-A2708D861F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B7230B-A979-3C44-AA2E-CBAC14D9932F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="1760" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B2A427CD-3A3B-AB4F-8475-A6742BF1F99B}"/>
+    <workbookView xWindow="2880" yWindow="1760" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B2A427CD-3A3B-AB4F-8475-A6742BF1F99B}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="Foglio5" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3403" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3407" uniqueCount="119">
   <si>
     <t>ds</t>
   </si>
@@ -393,6 +392,9 @@
   </si>
   <si>
     <t>categorical, missingValues, moreFeatures</t>
+  </si>
+  <si>
+    <t>labelAppend</t>
   </si>
 </sst>
 </file>
@@ -1656,8 +1658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{107DD696-A5A6-CB45-B2DD-8D2A6C9062E3}">
   <dimension ref="A1:J353"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="99" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2333,9 +2335,12 @@
         <v>22</v>
       </c>
       <c r="E31" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2630,9 +2635,12 @@
         <v>22</v>
       </c>
       <c r="E43" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2870,9 +2878,12 @@
         <v>22</v>
       </c>
       <c r="D55" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="F55" s="1" t="s">
         <v>85</v>
       </c>
       <c r="G55" s="1"/>
@@ -2891,12 +2902,14 @@
         <v>38</v>
       </c>
       <c r="E56" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="G56" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G56" s="1"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">

</xml_diff>

<commit_message>
- try auto sklearn
</commit_message>
<xml_diff>
--- a/DSBot/kb.xlsx
+++ b/DSBot/kb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarapido/Desktop/DSBot/DSBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82363679-251C-1B4C-B29B-FAA99F1E4BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C847A0F1-113E-AF42-A873-66B97660DEE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2980" yWindow="500" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B2A427CD-3A3B-AB4F-8475-A6742BF1F99B}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Foglio5" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Foglio2!$A$1:$J$474</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Foglio2!$A$1:$J$435</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -1737,10 +1737,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{107DD696-A5A6-CB45-B2DD-8D2A6C9062E3}">
-  <dimension ref="A1:J474"/>
+  <dimension ref="A1:J435"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="A429" sqref="A429:XFD480"/>
+    <sheetView tabSelected="1" topLeftCell="A367" zoomScale="99" workbookViewId="0">
+      <selection activeCell="A386" sqref="A386"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10531,7 +10531,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="385" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
         <v>15</v>
       </c>
@@ -10545,1465 +10545,1311 @@
         <v>20</v>
       </c>
     </row>
-    <row r="386" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D386" s="1"/>
-    </row>
-    <row r="387" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C387" s="1"/>
-      <c r="D387" s="1"/>
-    </row>
-    <row r="388" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B388" s="1"/>
-    </row>
-    <row r="389" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B389" s="1"/>
-      <c r="C389" s="1"/>
-    </row>
-    <row r="390" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B390" s="1"/>
-      <c r="D390" s="1"/>
-    </row>
-    <row r="391" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B391" s="1"/>
-      <c r="C391" s="1"/>
-      <c r="D391" s="1"/>
-    </row>
-    <row r="392" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C392" s="1"/>
-      <c r="D392" s="1"/>
-    </row>
-    <row r="393" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C393" s="1"/>
-      <c r="E393" s="1"/>
-    </row>
-    <row r="394" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C394" s="1"/>
-      <c r="D394" s="1"/>
-      <c r="E394" s="1"/>
-    </row>
-    <row r="395" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B395" s="1"/>
-      <c r="C395" s="1"/>
-    </row>
-    <row r="396" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C396" s="1"/>
-      <c r="D396" s="1"/>
-    </row>
-    <row r="397" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B397" s="1"/>
-      <c r="C397" s="1"/>
-    </row>
-    <row r="398" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B398" s="1"/>
-      <c r="C398" s="1"/>
-    </row>
-    <row r="399" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C399" s="1"/>
-    </row>
-    <row r="400" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D400" s="1"/>
-    </row>
-    <row r="401" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C401" s="1"/>
-      <c r="D401" s="1"/>
-    </row>
-    <row r="402" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B402" s="1"/>
-    </row>
-    <row r="403" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B403" s="1"/>
-      <c r="C403" s="1"/>
-    </row>
-    <row r="404" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B404" s="1"/>
-      <c r="D404" s="1"/>
-    </row>
-    <row r="405" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B405" s="1"/>
-      <c r="C405" s="1"/>
-      <c r="D405" s="1"/>
-    </row>
-    <row r="406" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C406" s="1"/>
-      <c r="D406" s="1"/>
-    </row>
-    <row r="407" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C407" s="1"/>
-      <c r="E407" s="1"/>
-    </row>
-    <row r="408" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C408" s="1"/>
-      <c r="D408" s="1"/>
-      <c r="E408" s="1"/>
-    </row>
-    <row r="409" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B409" s="1"/>
-      <c r="C409" s="1"/>
-    </row>
-    <row r="410" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C410" s="1"/>
-      <c r="D410" s="1"/>
-    </row>
-    <row r="411" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B411" s="1"/>
-      <c r="C411" s="1"/>
-    </row>
-    <row r="412" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B412" s="1"/>
-      <c r="C412" s="1"/>
-    </row>
-    <row r="413" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C413" s="1"/>
-    </row>
-    <row r="414" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D414" s="1"/>
-    </row>
-    <row r="415" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C415" s="1"/>
-      <c r="D415" s="1"/>
-    </row>
-    <row r="416" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B416" s="1"/>
-    </row>
-    <row r="417" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B417" s="1"/>
-      <c r="C417" s="1"/>
-    </row>
-    <row r="418" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B418" s="1"/>
-      <c r="D418" s="1"/>
-    </row>
-    <row r="419" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B419" s="1"/>
-      <c r="C419" s="1"/>
-      <c r="D419" s="1"/>
-    </row>
-    <row r="420" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C420" s="1"/>
-      <c r="D420" s="1"/>
-    </row>
-    <row r="421" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C421" s="1"/>
-      <c r="E421" s="1"/>
-    </row>
-    <row r="422" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C422" s="1"/>
-      <c r="D422" s="1"/>
-      <c r="E422" s="1"/>
-    </row>
-    <row r="423" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B423" s="1"/>
-      <c r="C423" s="1"/>
-    </row>
-    <row r="424" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C424" s="1"/>
-      <c r="D424" s="1"/>
-    </row>
-    <row r="425" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A386" t="s">
+        <v>47</v>
+      </c>
+      <c r="B386" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C386" t="s">
+        <v>67</v>
+      </c>
+      <c r="D386" t="s">
+        <v>144</v>
+      </c>
+      <c r="E386" t="s">
+        <v>79</v>
+      </c>
+      <c r="F386" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="387" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A387" t="s">
+        <v>47</v>
+      </c>
+      <c r="B387" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C387" t="s">
+        <v>67</v>
+      </c>
+      <c r="D387" t="s">
+        <v>144</v>
+      </c>
+      <c r="E387" t="s">
+        <v>118</v>
+      </c>
+      <c r="F387" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="388" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A388" t="s">
+        <v>61</v>
+      </c>
+      <c r="B388" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C388" t="s">
+        <v>67</v>
+      </c>
+      <c r="D388" t="s">
+        <v>144</v>
+      </c>
+      <c r="E388" t="s">
+        <v>79</v>
+      </c>
+      <c r="F388" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="389" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A389" t="s">
+        <v>61</v>
+      </c>
+      <c r="B389" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C389" t="s">
+        <v>67</v>
+      </c>
+      <c r="D389" t="s">
+        <v>144</v>
+      </c>
+      <c r="E389" t="s">
+        <v>118</v>
+      </c>
+      <c r="F389" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="390" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A390" t="s">
+        <v>49</v>
+      </c>
+      <c r="B390" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C390" t="s">
+        <v>22</v>
+      </c>
+      <c r="D390" t="s">
+        <v>67</v>
+      </c>
+      <c r="E390" t="s">
+        <v>144</v>
+      </c>
+      <c r="F390" t="s">
+        <v>79</v>
+      </c>
+      <c r="G390" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="391" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A391" t="s">
+        <v>49</v>
+      </c>
+      <c r="B391" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C391" t="s">
+        <v>22</v>
+      </c>
+      <c r="D391" t="s">
+        <v>67</v>
+      </c>
+      <c r="E391" t="s">
+        <v>144</v>
+      </c>
+      <c r="F391" t="s">
+        <v>118</v>
+      </c>
+      <c r="G391" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="392" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A392" t="s">
+        <v>94</v>
+      </c>
+      <c r="B392" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C392" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D392" t="s">
+        <v>67</v>
+      </c>
+      <c r="E392" t="s">
+        <v>144</v>
+      </c>
+      <c r="F392" t="s">
+        <v>79</v>
+      </c>
+      <c r="G392" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="393" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A393" t="s">
+        <v>94</v>
+      </c>
+      <c r="B393" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C393" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D393" t="s">
+        <v>67</v>
+      </c>
+      <c r="E393" t="s">
+        <v>144</v>
+      </c>
+      <c r="F393" t="s">
+        <v>118</v>
+      </c>
+      <c r="G393" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="394" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A394" t="s">
+        <v>47</v>
+      </c>
+      <c r="B394" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C394" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D394" t="s">
+        <v>67</v>
+      </c>
+      <c r="E394" t="s">
+        <v>144</v>
+      </c>
+      <c r="F394" t="s">
+        <v>79</v>
+      </c>
+      <c r="G394" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="395" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A395" t="s">
+        <v>47</v>
+      </c>
+      <c r="B395" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C395" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D395" t="s">
+        <v>67</v>
+      </c>
+      <c r="E395" t="s">
+        <v>144</v>
+      </c>
+      <c r="F395" t="s">
+        <v>118</v>
+      </c>
+      <c r="G395" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="396" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A396" t="s">
+        <v>61</v>
+      </c>
+      <c r="B396" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C396" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D396" t="s">
+        <v>67</v>
+      </c>
+      <c r="E396" t="s">
+        <v>144</v>
+      </c>
+      <c r="F396" t="s">
+        <v>79</v>
+      </c>
+      <c r="G396" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="397" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A397" t="s">
+        <v>61</v>
+      </c>
+      <c r="B397" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C397" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D397" t="s">
+        <v>67</v>
+      </c>
+      <c r="E397" t="s">
+        <v>144</v>
+      </c>
+      <c r="F397" t="s">
+        <v>118</v>
+      </c>
+      <c r="G397" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="398" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A398" t="s">
+        <v>61</v>
+      </c>
+      <c r="B398" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C398" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D398" t="s">
+        <v>67</v>
+      </c>
+      <c r="E398" t="s">
+        <v>144</v>
+      </c>
+      <c r="F398" t="s">
+        <v>79</v>
+      </c>
+      <c r="G398" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="399" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A399" t="s">
+        <v>61</v>
+      </c>
+      <c r="B399" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C399" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D399" t="s">
+        <v>67</v>
+      </c>
+      <c r="E399" t="s">
+        <v>144</v>
+      </c>
+      <c r="F399" t="s">
+        <v>118</v>
+      </c>
+      <c r="G399" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="400" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A400" t="s">
+        <v>111</v>
+      </c>
+      <c r="B400" t="s">
+        <v>11</v>
+      </c>
+      <c r="C400" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D400" t="s">
+        <v>67</v>
+      </c>
+      <c r="E400" t="s">
+        <v>144</v>
+      </c>
+      <c r="F400" t="s">
+        <v>79</v>
+      </c>
+      <c r="G400" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="401" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A401" t="s">
+        <v>111</v>
+      </c>
+      <c r="B401" t="s">
+        <v>11</v>
+      </c>
+      <c r="C401" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D401" t="s">
+        <v>67</v>
+      </c>
+      <c r="E401" t="s">
+        <v>144</v>
+      </c>
+      <c r="F401" t="s">
+        <v>118</v>
+      </c>
+      <c r="G401" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="402" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A402" t="s">
+        <v>89</v>
+      </c>
+      <c r="B402" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C402" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D402" t="s">
+        <v>22</v>
+      </c>
+      <c r="E402" t="s">
+        <v>67</v>
+      </c>
+      <c r="F402" t="s">
+        <v>144</v>
+      </c>
+      <c r="G402" t="s">
+        <v>79</v>
+      </c>
+      <c r="H402" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="403" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A403" t="s">
+        <v>89</v>
+      </c>
+      <c r="B403" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C403" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D403" t="s">
+        <v>22</v>
+      </c>
+      <c r="E403" t="s">
+        <v>67</v>
+      </c>
+      <c r="F403" t="s">
+        <v>144</v>
+      </c>
+      <c r="G403" t="s">
+        <v>118</v>
+      </c>
+      <c r="H403" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="404" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A404" t="s">
+        <v>49</v>
+      </c>
+      <c r="B404" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C404" t="s">
+        <v>22</v>
+      </c>
+      <c r="D404" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E404" t="s">
+        <v>67</v>
+      </c>
+      <c r="F404" t="s">
+        <v>144</v>
+      </c>
+      <c r="G404" t="s">
+        <v>79</v>
+      </c>
+      <c r="H404" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="405" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A405" t="s">
+        <v>49</v>
+      </c>
+      <c r="B405" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C405" t="s">
+        <v>22</v>
+      </c>
+      <c r="D405" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E405" t="s">
+        <v>67</v>
+      </c>
+      <c r="F405" t="s">
+        <v>144</v>
+      </c>
+      <c r="G405" t="s">
+        <v>118</v>
+      </c>
+      <c r="H405" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="406" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A406" t="s">
+        <v>63</v>
+      </c>
+      <c r="B406" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C406" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D406" t="s">
+        <v>22</v>
+      </c>
+      <c r="E406" t="s">
+        <v>67</v>
+      </c>
+      <c r="F406" t="s">
+        <v>144</v>
+      </c>
+      <c r="G406" t="s">
+        <v>79</v>
+      </c>
+      <c r="H406" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="407" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A407" t="s">
+        <v>63</v>
+      </c>
+      <c r="B407" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C407" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D407" t="s">
+        <v>22</v>
+      </c>
+      <c r="E407" t="s">
+        <v>67</v>
+      </c>
+      <c r="F407" t="s">
+        <v>144</v>
+      </c>
+      <c r="G407" t="s">
+        <v>118</v>
+      </c>
+      <c r="H407" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="408" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A408" t="s">
+        <v>94</v>
+      </c>
+      <c r="B408" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C408" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D408" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E408" t="s">
+        <v>67</v>
+      </c>
+      <c r="F408" t="s">
+        <v>144</v>
+      </c>
+      <c r="G408" t="s">
+        <v>79</v>
+      </c>
+      <c r="H408" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="409" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A409" t="s">
+        <v>94</v>
+      </c>
+      <c r="B409" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C409" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D409" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E409" t="s">
+        <v>67</v>
+      </c>
+      <c r="F409" t="s">
+        <v>144</v>
+      </c>
+      <c r="G409" t="s">
+        <v>118</v>
+      </c>
+      <c r="H409" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="410" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A410" t="s">
+        <v>95</v>
+      </c>
+      <c r="B410" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C410" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D410" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E410" t="s">
+        <v>67</v>
+      </c>
+      <c r="F410" t="s">
+        <v>144</v>
+      </c>
+      <c r="G410" t="s">
+        <v>79</v>
+      </c>
+      <c r="H410" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="411" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A411" t="s">
+        <v>95</v>
+      </c>
+      <c r="B411" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C411" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D411" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E411" t="s">
+        <v>67</v>
+      </c>
+      <c r="F411" t="s">
+        <v>144</v>
+      </c>
+      <c r="G411" t="s">
+        <v>118</v>
+      </c>
+      <c r="H411" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="412" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A412" t="s">
+        <v>104</v>
+      </c>
+      <c r="B412" t="s">
+        <v>11</v>
+      </c>
+      <c r="C412" t="s">
+        <v>69</v>
+      </c>
+      <c r="D412" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E412" t="s">
+        <v>67</v>
+      </c>
+      <c r="F412" t="s">
+        <v>144</v>
+      </c>
+      <c r="G412" t="s">
+        <v>79</v>
+      </c>
+      <c r="H412" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="413" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A413" t="s">
+        <v>104</v>
+      </c>
+      <c r="B413" t="s">
+        <v>11</v>
+      </c>
+      <c r="C413" t="s">
+        <v>69</v>
+      </c>
+      <c r="D413" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E413" t="s">
+        <v>67</v>
+      </c>
+      <c r="F413" t="s">
+        <v>144</v>
+      </c>
+      <c r="G413" t="s">
+        <v>118</v>
+      </c>
+      <c r="H413" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="414" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A414" t="s">
+        <v>61</v>
+      </c>
+      <c r="B414" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C414" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D414" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E414" t="s">
+        <v>67</v>
+      </c>
+      <c r="F414" t="s">
+        <v>144</v>
+      </c>
+      <c r="G414" t="s">
+        <v>79</v>
+      </c>
+      <c r="H414" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="415" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A415" t="s">
+        <v>61</v>
+      </c>
+      <c r="B415" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C415" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D415" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E415" t="s">
+        <v>67</v>
+      </c>
+      <c r="F415" t="s">
+        <v>144</v>
+      </c>
+      <c r="G415" t="s">
+        <v>118</v>
+      </c>
+      <c r="H415" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="416" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A416" t="s">
+        <v>112</v>
+      </c>
+      <c r="B416" t="s">
+        <v>11</v>
+      </c>
+      <c r="C416" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D416" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E416" t="s">
+        <v>67</v>
+      </c>
+      <c r="F416" t="s">
+        <v>144</v>
+      </c>
+      <c r="G416" t="s">
+        <v>79</v>
+      </c>
+      <c r="H416" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="417" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A417" t="s">
+        <v>112</v>
+      </c>
+      <c r="B417" t="s">
+        <v>11</v>
+      </c>
+      <c r="C417" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D417" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E417" t="s">
+        <v>67</v>
+      </c>
+      <c r="F417" t="s">
+        <v>144</v>
+      </c>
+      <c r="G417" t="s">
+        <v>118</v>
+      </c>
+      <c r="H417" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="418" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A418" t="s">
+        <v>111</v>
+      </c>
+      <c r="B418" t="s">
+        <v>11</v>
+      </c>
+      <c r="C418" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D418" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E418" t="s">
+        <v>67</v>
+      </c>
+      <c r="F418" t="s">
+        <v>144</v>
+      </c>
+      <c r="G418" t="s">
+        <v>79</v>
+      </c>
+      <c r="H418" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="419" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A419" t="s">
+        <v>111</v>
+      </c>
+      <c r="B419" t="s">
+        <v>11</v>
+      </c>
+      <c r="C419" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D419" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E419" t="s">
+        <v>67</v>
+      </c>
+      <c r="F419" t="s">
+        <v>144</v>
+      </c>
+      <c r="G419" t="s">
+        <v>118</v>
+      </c>
+      <c r="H419" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="420" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A420" t="s">
+        <v>89</v>
+      </c>
+      <c r="B420" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C420" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D420" t="s">
+        <v>22</v>
+      </c>
+      <c r="E420" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F420" t="s">
+        <v>67</v>
+      </c>
+      <c r="G420" t="s">
+        <v>144</v>
+      </c>
+      <c r="H420" t="s">
+        <v>79</v>
+      </c>
+      <c r="I420" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="421" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A421" t="s">
+        <v>89</v>
+      </c>
+      <c r="B421" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C421" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D421" t="s">
+        <v>22</v>
+      </c>
+      <c r="E421" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F421" t="s">
+        <v>67</v>
+      </c>
+      <c r="G421" t="s">
+        <v>144</v>
+      </c>
+      <c r="H421" t="s">
+        <v>118</v>
+      </c>
+      <c r="I421" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="422" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A422" t="s">
+        <v>90</v>
+      </c>
+      <c r="B422" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C422" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D422" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E422" t="s">
+        <v>22</v>
+      </c>
+      <c r="F422" t="s">
+        <v>67</v>
+      </c>
+      <c r="G422" t="s">
+        <v>144</v>
+      </c>
+      <c r="H422" t="s">
+        <v>79</v>
+      </c>
+      <c r="I422" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="423" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A423" t="s">
+        <v>90</v>
+      </c>
+      <c r="B423" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C423" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D423" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E423" t="s">
+        <v>22</v>
+      </c>
+      <c r="F423" t="s">
+        <v>67</v>
+      </c>
+      <c r="G423" t="s">
+        <v>144</v>
+      </c>
+      <c r="H423" t="s">
+        <v>118</v>
+      </c>
+      <c r="I423" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="424" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A424" t="s">
+        <v>63</v>
+      </c>
+      <c r="B424" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C424" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D424" t="s">
+        <v>22</v>
+      </c>
+      <c r="E424" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F424" t="s">
+        <v>67</v>
+      </c>
+      <c r="G424" t="s">
+        <v>144</v>
+      </c>
+      <c r="H424" t="s">
+        <v>79</v>
+      </c>
+      <c r="I424" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="425" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A425" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="B425" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C425" t="s">
-        <v>67</v>
+      <c r="C425" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="D425" t="s">
+        <v>22</v>
+      </c>
+      <c r="E425" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F425" t="s">
+        <v>67</v>
+      </c>
+      <c r="G425" t="s">
         <v>144</v>
       </c>
-      <c r="E425" t="s">
+      <c r="H425" t="s">
+        <v>118</v>
+      </c>
+      <c r="I425" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="426" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A426" t="s">
+        <v>95</v>
+      </c>
+      <c r="B426" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C426" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D426" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E426" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F426" t="s">
+        <v>67</v>
+      </c>
+      <c r="G426" t="s">
+        <v>144</v>
+      </c>
+      <c r="H426" t="s">
+        <v>118</v>
+      </c>
+      <c r="I426" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="427" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A427" t="s">
+        <v>95</v>
+      </c>
+      <c r="B427" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C427" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D427" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E427" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F427" t="s">
+        <v>67</v>
+      </c>
+      <c r="G427" t="s">
+        <v>144</v>
+      </c>
+      <c r="H427" t="s">
         <v>79</v>
       </c>
-      <c r="F425" t="s">
+      <c r="I427" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="426" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A426" t="s">
-        <v>47</v>
-      </c>
-      <c r="B426" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C426" t="s">
-        <v>67</v>
-      </c>
-      <c r="D426" t="s">
+    <row r="428" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A428" t="s">
+        <v>105</v>
+      </c>
+      <c r="B428" t="s">
+        <v>11</v>
+      </c>
+      <c r="C428" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D428" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E428" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F428" t="s">
+        <v>67</v>
+      </c>
+      <c r="G428" t="s">
         <v>144</v>
       </c>
-      <c r="E426" t="s">
+      <c r="H428" t="s">
+        <v>79</v>
+      </c>
+      <c r="I428" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="429" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A429" t="s">
+        <v>105</v>
+      </c>
+      <c r="B429" t="s">
+        <v>11</v>
+      </c>
+      <c r="C429" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D429" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E429" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F429" t="s">
+        <v>67</v>
+      </c>
+      <c r="G429" t="s">
+        <v>144</v>
+      </c>
+      <c r="H429" t="s">
         <v>118</v>
       </c>
-      <c r="F426" t="s">
+      <c r="I429" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="427" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A427" t="s">
-        <v>61</v>
-      </c>
-      <c r="B427" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C427" t="s">
-        <v>67</v>
-      </c>
-      <c r="D427" t="s">
+    <row r="430" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A430" t="s">
+        <v>104</v>
+      </c>
+      <c r="B430" t="s">
+        <v>11</v>
+      </c>
+      <c r="C430" t="s">
+        <v>69</v>
+      </c>
+      <c r="D430" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E430" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F430" t="s">
+        <v>67</v>
+      </c>
+      <c r="G430" t="s">
         <v>144</v>
       </c>
-      <c r="E427" t="s">
+      <c r="H430" t="s">
         <v>79</v>
       </c>
-      <c r="F427" t="s">
+      <c r="I430" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="428" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A428" t="s">
-        <v>61</v>
-      </c>
-      <c r="B428" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C428" t="s">
-        <v>67</v>
-      </c>
-      <c r="D428" t="s">
+    <row r="431" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A431" t="s">
+        <v>104</v>
+      </c>
+      <c r="B431" t="s">
+        <v>11</v>
+      </c>
+      <c r="C431" t="s">
+        <v>69</v>
+      </c>
+      <c r="D431" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E431" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F431" t="s">
+        <v>67</v>
+      </c>
+      <c r="G431" t="s">
         <v>144</v>
       </c>
-      <c r="E428" t="s">
+      <c r="H431" t="s">
         <v>118</v>
       </c>
-      <c r="F428" t="s">
+      <c r="I431" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="429" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A429" t="s">
-        <v>49</v>
-      </c>
-      <c r="B429" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C429" t="s">
-        <v>22</v>
-      </c>
-      <c r="D429" t="s">
-        <v>67</v>
-      </c>
-      <c r="E429" t="s">
+    <row r="432" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A432" t="s">
+        <v>112</v>
+      </c>
+      <c r="B432" t="s">
+        <v>11</v>
+      </c>
+      <c r="C432" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D432" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E432" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F432" t="s">
+        <v>67</v>
+      </c>
+      <c r="G432" t="s">
         <v>144</v>
       </c>
-      <c r="F429" t="s">
+      <c r="H432" t="s">
         <v>79</v>
       </c>
-      <c r="G429" t="s">
+      <c r="I432" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="430" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A430" t="s">
-        <v>49</v>
-      </c>
-      <c r="B430" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C430" t="s">
-        <v>22</v>
-      </c>
-      <c r="D430" t="s">
-        <v>67</v>
-      </c>
-      <c r="E430" t="s">
+    <row r="433" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A433" t="s">
+        <v>112</v>
+      </c>
+      <c r="B433" t="s">
+        <v>11</v>
+      </c>
+      <c r="C433" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D433" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E433" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F433" t="s">
+        <v>67</v>
+      </c>
+      <c r="G433" t="s">
         <v>144</v>
       </c>
-      <c r="F430" t="s">
+      <c r="H433" t="s">
         <v>118</v>
       </c>
-      <c r="G430" t="s">
+      <c r="I433" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="431" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A431" t="s">
-        <v>94</v>
-      </c>
-      <c r="B431" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C431" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D431" t="s">
-        <v>67</v>
-      </c>
-      <c r="E431" t="s">
+    <row r="434" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A434" t="s">
+        <v>105</v>
+      </c>
+      <c r="B434" t="s">
+        <v>11</v>
+      </c>
+      <c r="C434" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D434" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E434" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F434" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G434" t="s">
+        <v>67</v>
+      </c>
+      <c r="H434" t="s">
         <v>144</v>
       </c>
-      <c r="F431" t="s">
+      <c r="I434" t="s">
         <v>79</v>
       </c>
-      <c r="G431" t="s">
+      <c r="J434" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="432" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A432" t="s">
-        <v>94</v>
-      </c>
-      <c r="B432" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C432" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D432" t="s">
-        <v>67</v>
-      </c>
-      <c r="E432" t="s">
+    <row r="435" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A435" t="s">
+        <v>105</v>
+      </c>
+      <c r="B435" t="s">
+        <v>11</v>
+      </c>
+      <c r="C435" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D435" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E435" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F435" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G435" t="s">
+        <v>67</v>
+      </c>
+      <c r="H435" t="s">
         <v>144</v>
       </c>
-      <c r="F432" t="s">
+      <c r="I435" t="s">
         <v>118</v>
       </c>
-      <c r="G432" t="s">
+      <c r="J435" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="433" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A433" t="s">
-        <v>47</v>
-      </c>
-      <c r="B433" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C433" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D433" t="s">
-        <v>67</v>
-      </c>
-      <c r="E433" t="s">
-        <v>144</v>
-      </c>
-      <c r="F433" t="s">
-        <v>79</v>
-      </c>
-      <c r="G433" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="434" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A434" t="s">
-        <v>47</v>
-      </c>
-      <c r="B434" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C434" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D434" t="s">
-        <v>67</v>
-      </c>
-      <c r="E434" t="s">
-        <v>144</v>
-      </c>
-      <c r="F434" t="s">
-        <v>118</v>
-      </c>
-      <c r="G434" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="435" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A435" t="s">
-        <v>61</v>
-      </c>
-      <c r="B435" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C435" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D435" t="s">
-        <v>67</v>
-      </c>
-      <c r="E435" t="s">
-        <v>144</v>
-      </c>
-      <c r="F435" t="s">
-        <v>79</v>
-      </c>
-      <c r="G435" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="436" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A436" t="s">
-        <v>61</v>
-      </c>
-      <c r="B436" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C436" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D436" t="s">
-        <v>67</v>
-      </c>
-      <c r="E436" t="s">
-        <v>144</v>
-      </c>
-      <c r="F436" t="s">
-        <v>118</v>
-      </c>
-      <c r="G436" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="437" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A437" t="s">
-        <v>61</v>
-      </c>
-      <c r="B437" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C437" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D437" t="s">
-        <v>67</v>
-      </c>
-      <c r="E437" t="s">
-        <v>144</v>
-      </c>
-      <c r="F437" t="s">
-        <v>79</v>
-      </c>
-      <c r="G437" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="438" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A438" t="s">
-        <v>61</v>
-      </c>
-      <c r="B438" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C438" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D438" t="s">
-        <v>67</v>
-      </c>
-      <c r="E438" t="s">
-        <v>144</v>
-      </c>
-      <c r="F438" t="s">
-        <v>118</v>
-      </c>
-      <c r="G438" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="439" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A439" t="s">
-        <v>111</v>
-      </c>
-      <c r="B439" t="s">
-        <v>11</v>
-      </c>
-      <c r="C439" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D439" t="s">
-        <v>67</v>
-      </c>
-      <c r="E439" t="s">
-        <v>144</v>
-      </c>
-      <c r="F439" t="s">
-        <v>79</v>
-      </c>
-      <c r="G439" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="440" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A440" t="s">
-        <v>111</v>
-      </c>
-      <c r="B440" t="s">
-        <v>11</v>
-      </c>
-      <c r="C440" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D440" t="s">
-        <v>67</v>
-      </c>
-      <c r="E440" t="s">
-        <v>144</v>
-      </c>
-      <c r="F440" t="s">
-        <v>118</v>
-      </c>
-      <c r="G440" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="441" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A441" t="s">
-        <v>89</v>
-      </c>
-      <c r="B441" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C441" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D441" t="s">
-        <v>22</v>
-      </c>
-      <c r="E441" t="s">
-        <v>67</v>
-      </c>
-      <c r="F441" t="s">
-        <v>144</v>
-      </c>
-      <c r="G441" t="s">
-        <v>79</v>
-      </c>
-      <c r="H441" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="442" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A442" t="s">
-        <v>89</v>
-      </c>
-      <c r="B442" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C442" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D442" t="s">
-        <v>22</v>
-      </c>
-      <c r="E442" t="s">
-        <v>67</v>
-      </c>
-      <c r="F442" t="s">
-        <v>144</v>
-      </c>
-      <c r="G442" t="s">
-        <v>118</v>
-      </c>
-      <c r="H442" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="443" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A443" t="s">
-        <v>49</v>
-      </c>
-      <c r="B443" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C443" t="s">
-        <v>22</v>
-      </c>
-      <c r="D443" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E443" t="s">
-        <v>67</v>
-      </c>
-      <c r="F443" t="s">
-        <v>144</v>
-      </c>
-      <c r="G443" t="s">
-        <v>79</v>
-      </c>
-      <c r="H443" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="444" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A444" t="s">
-        <v>49</v>
-      </c>
-      <c r="B444" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C444" t="s">
-        <v>22</v>
-      </c>
-      <c r="D444" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E444" t="s">
-        <v>67</v>
-      </c>
-      <c r="F444" t="s">
-        <v>144</v>
-      </c>
-      <c r="G444" t="s">
-        <v>118</v>
-      </c>
-      <c r="H444" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="445" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A445" t="s">
-        <v>63</v>
-      </c>
-      <c r="B445" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C445" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D445" t="s">
-        <v>22</v>
-      </c>
-      <c r="E445" t="s">
-        <v>67</v>
-      </c>
-      <c r="F445" t="s">
-        <v>144</v>
-      </c>
-      <c r="G445" t="s">
-        <v>79</v>
-      </c>
-      <c r="H445" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="446" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A446" t="s">
-        <v>63</v>
-      </c>
-      <c r="B446" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C446" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D446" t="s">
-        <v>22</v>
-      </c>
-      <c r="E446" t="s">
-        <v>67</v>
-      </c>
-      <c r="F446" t="s">
-        <v>144</v>
-      </c>
-      <c r="G446" t="s">
-        <v>118</v>
-      </c>
-      <c r="H446" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="447" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A447" t="s">
-        <v>94</v>
-      </c>
-      <c r="B447" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C447" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D447" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E447" t="s">
-        <v>67</v>
-      </c>
-      <c r="F447" t="s">
-        <v>144</v>
-      </c>
-      <c r="G447" t="s">
-        <v>79</v>
-      </c>
-      <c r="H447" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="448" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A448" t="s">
-        <v>94</v>
-      </c>
-      <c r="B448" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C448" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D448" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E448" t="s">
-        <v>67</v>
-      </c>
-      <c r="F448" t="s">
-        <v>144</v>
-      </c>
-      <c r="G448" t="s">
-        <v>118</v>
-      </c>
-      <c r="H448" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="449" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A449" t="s">
-        <v>95</v>
-      </c>
-      <c r="B449" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C449" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D449" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E449" t="s">
-        <v>67</v>
-      </c>
-      <c r="F449" t="s">
-        <v>144</v>
-      </c>
-      <c r="G449" t="s">
-        <v>79</v>
-      </c>
-      <c r="H449" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="450" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A450" t="s">
-        <v>95</v>
-      </c>
-      <c r="B450" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C450" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D450" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E450" t="s">
-        <v>67</v>
-      </c>
-      <c r="F450" t="s">
-        <v>144</v>
-      </c>
-      <c r="G450" t="s">
-        <v>118</v>
-      </c>
-      <c r="H450" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="451" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A451" t="s">
-        <v>104</v>
-      </c>
-      <c r="B451" t="s">
-        <v>11</v>
-      </c>
-      <c r="C451" t="s">
-        <v>69</v>
-      </c>
-      <c r="D451" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E451" t="s">
-        <v>67</v>
-      </c>
-      <c r="F451" t="s">
-        <v>144</v>
-      </c>
-      <c r="G451" t="s">
-        <v>79</v>
-      </c>
-      <c r="H451" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="452" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A452" t="s">
-        <v>104</v>
-      </c>
-      <c r="B452" t="s">
-        <v>11</v>
-      </c>
-      <c r="C452" t="s">
-        <v>69</v>
-      </c>
-      <c r="D452" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E452" t="s">
-        <v>67</v>
-      </c>
-      <c r="F452" t="s">
-        <v>144</v>
-      </c>
-      <c r="G452" t="s">
-        <v>118</v>
-      </c>
-      <c r="H452" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="453" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A453" t="s">
-        <v>61</v>
-      </c>
-      <c r="B453" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C453" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D453" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E453" t="s">
-        <v>67</v>
-      </c>
-      <c r="F453" t="s">
-        <v>144</v>
-      </c>
-      <c r="G453" t="s">
-        <v>79</v>
-      </c>
-      <c r="H453" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="454" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A454" t="s">
-        <v>61</v>
-      </c>
-      <c r="B454" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C454" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D454" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E454" t="s">
-        <v>67</v>
-      </c>
-      <c r="F454" t="s">
-        <v>144</v>
-      </c>
-      <c r="G454" t="s">
-        <v>118</v>
-      </c>
-      <c r="H454" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="455" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A455" t="s">
-        <v>112</v>
-      </c>
-      <c r="B455" t="s">
-        <v>11</v>
-      </c>
-      <c r="C455" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D455" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E455" t="s">
-        <v>67</v>
-      </c>
-      <c r="F455" t="s">
-        <v>144</v>
-      </c>
-      <c r="G455" t="s">
-        <v>79</v>
-      </c>
-      <c r="H455" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="456" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A456" t="s">
-        <v>112</v>
-      </c>
-      <c r="B456" t="s">
-        <v>11</v>
-      </c>
-      <c r="C456" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D456" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E456" t="s">
-        <v>67</v>
-      </c>
-      <c r="F456" t="s">
-        <v>144</v>
-      </c>
-      <c r="G456" t="s">
-        <v>118</v>
-      </c>
-      <c r="H456" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="457" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A457" t="s">
-        <v>111</v>
-      </c>
-      <c r="B457" t="s">
-        <v>11</v>
-      </c>
-      <c r="C457" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D457" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E457" t="s">
-        <v>67</v>
-      </c>
-      <c r="F457" t="s">
-        <v>144</v>
-      </c>
-      <c r="G457" t="s">
-        <v>79</v>
-      </c>
-      <c r="H457" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="458" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A458" t="s">
-        <v>111</v>
-      </c>
-      <c r="B458" t="s">
-        <v>11</v>
-      </c>
-      <c r="C458" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D458" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E458" t="s">
-        <v>67</v>
-      </c>
-      <c r="F458" t="s">
-        <v>144</v>
-      </c>
-      <c r="G458" t="s">
-        <v>118</v>
-      </c>
-      <c r="H458" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="459" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A459" t="s">
-        <v>89</v>
-      </c>
-      <c r="B459" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C459" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D459" t="s">
-        <v>22</v>
-      </c>
-      <c r="E459" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F459" t="s">
-        <v>67</v>
-      </c>
-      <c r="G459" t="s">
-        <v>144</v>
-      </c>
-      <c r="H459" t="s">
-        <v>79</v>
-      </c>
-      <c r="I459" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="460" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A460" t="s">
-        <v>89</v>
-      </c>
-      <c r="B460" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C460" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D460" t="s">
-        <v>22</v>
-      </c>
-      <c r="E460" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F460" t="s">
-        <v>67</v>
-      </c>
-      <c r="G460" t="s">
-        <v>144</v>
-      </c>
-      <c r="H460" t="s">
-        <v>118</v>
-      </c>
-      <c r="I460" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="461" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A461" t="s">
-        <v>90</v>
-      </c>
-      <c r="B461" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C461" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D461" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E461" t="s">
-        <v>22</v>
-      </c>
-      <c r="F461" t="s">
-        <v>67</v>
-      </c>
-      <c r="G461" t="s">
-        <v>144</v>
-      </c>
-      <c r="H461" t="s">
-        <v>79</v>
-      </c>
-      <c r="I461" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="462" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A462" t="s">
-        <v>90</v>
-      </c>
-      <c r="B462" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C462" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D462" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E462" t="s">
-        <v>22</v>
-      </c>
-      <c r="F462" t="s">
-        <v>67</v>
-      </c>
-      <c r="G462" t="s">
-        <v>144</v>
-      </c>
-      <c r="H462" t="s">
-        <v>118</v>
-      </c>
-      <c r="I462" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="463" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A463" t="s">
-        <v>63</v>
-      </c>
-      <c r="B463" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C463" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D463" t="s">
-        <v>22</v>
-      </c>
-      <c r="E463" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F463" t="s">
-        <v>67</v>
-      </c>
-      <c r="G463" t="s">
-        <v>144</v>
-      </c>
-      <c r="H463" t="s">
-        <v>79</v>
-      </c>
-      <c r="I463" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="464" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A464" t="s">
-        <v>63</v>
-      </c>
-      <c r="B464" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C464" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D464" t="s">
-        <v>22</v>
-      </c>
-      <c r="E464" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F464" t="s">
-        <v>67</v>
-      </c>
-      <c r="G464" t="s">
-        <v>144</v>
-      </c>
-      <c r="H464" t="s">
-        <v>118</v>
-      </c>
-      <c r="I464" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="465" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A465" t="s">
-        <v>95</v>
-      </c>
-      <c r="B465" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C465" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D465" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E465" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F465" t="s">
-        <v>67</v>
-      </c>
-      <c r="G465" t="s">
-        <v>144</v>
-      </c>
-      <c r="H465" t="s">
-        <v>118</v>
-      </c>
-      <c r="I465" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="466" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A466" t="s">
-        <v>95</v>
-      </c>
-      <c r="B466" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C466" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D466" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E466" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F466" t="s">
-        <v>67</v>
-      </c>
-      <c r="G466" t="s">
-        <v>144</v>
-      </c>
-      <c r="H466" t="s">
-        <v>79</v>
-      </c>
-      <c r="I466" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="467" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A467" t="s">
-        <v>105</v>
-      </c>
-      <c r="B467" t="s">
-        <v>11</v>
-      </c>
-      <c r="C467" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D467" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E467" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F467" t="s">
-        <v>67</v>
-      </c>
-      <c r="G467" t="s">
-        <v>144</v>
-      </c>
-      <c r="H467" t="s">
-        <v>79</v>
-      </c>
-      <c r="I467" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="468" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A468" t="s">
-        <v>105</v>
-      </c>
-      <c r="B468" t="s">
-        <v>11</v>
-      </c>
-      <c r="C468" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D468" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E468" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F468" t="s">
-        <v>67</v>
-      </c>
-      <c r="G468" t="s">
-        <v>144</v>
-      </c>
-      <c r="H468" t="s">
-        <v>118</v>
-      </c>
-      <c r="I468" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="469" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A469" t="s">
-        <v>104</v>
-      </c>
-      <c r="B469" t="s">
-        <v>11</v>
-      </c>
-      <c r="C469" t="s">
-        <v>69</v>
-      </c>
-      <c r="D469" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E469" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F469" t="s">
-        <v>67</v>
-      </c>
-      <c r="G469" t="s">
-        <v>144</v>
-      </c>
-      <c r="H469" t="s">
-        <v>79</v>
-      </c>
-      <c r="I469" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="470" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A470" t="s">
-        <v>104</v>
-      </c>
-      <c r="B470" t="s">
-        <v>11</v>
-      </c>
-      <c r="C470" t="s">
-        <v>69</v>
-      </c>
-      <c r="D470" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E470" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F470" t="s">
-        <v>67</v>
-      </c>
-      <c r="G470" t="s">
-        <v>144</v>
-      </c>
-      <c r="H470" t="s">
-        <v>118</v>
-      </c>
-      <c r="I470" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="471" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A471" t="s">
-        <v>112</v>
-      </c>
-      <c r="B471" t="s">
-        <v>11</v>
-      </c>
-      <c r="C471" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D471" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E471" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F471" t="s">
-        <v>67</v>
-      </c>
-      <c r="G471" t="s">
-        <v>144</v>
-      </c>
-      <c r="H471" t="s">
-        <v>79</v>
-      </c>
-      <c r="I471" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="472" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A472" t="s">
-        <v>112</v>
-      </c>
-      <c r="B472" t="s">
-        <v>11</v>
-      </c>
-      <c r="C472" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D472" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E472" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F472" t="s">
-        <v>67</v>
-      </c>
-      <c r="G472" t="s">
-        <v>144</v>
-      </c>
-      <c r="H472" t="s">
-        <v>118</v>
-      </c>
-      <c r="I472" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="473" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A473" t="s">
-        <v>105</v>
-      </c>
-      <c r="B473" t="s">
-        <v>11</v>
-      </c>
-      <c r="C473" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D473" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E473" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F473" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G473" t="s">
-        <v>67</v>
-      </c>
-      <c r="H473" t="s">
-        <v>144</v>
-      </c>
-      <c r="I473" t="s">
-        <v>79</v>
-      </c>
-      <c r="J473" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="474" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A474" t="s">
-        <v>105</v>
-      </c>
-      <c r="B474" t="s">
-        <v>11</v>
-      </c>
-      <c r="C474" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D474" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E474" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F474" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G474" t="s">
-        <v>67</v>
-      </c>
-      <c r="H474" t="s">
-        <v>144</v>
-      </c>
-      <c r="I474" t="s">
-        <v>118</v>
-      </c>
-      <c r="J474" t="s">
-        <v>119</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:J474" xr:uid="{107DD696-A5A6-CB45-B2DD-8D2A6C9062E3}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:J428">
-    <sortCondition ref="A1:A428"/>
-    <sortCondition ref="B1:B428"/>
-    <sortCondition ref="C1:C428"/>
-    <sortCondition ref="D1:D428"/>
-    <sortCondition ref="E1:E428"/>
-    <sortCondition ref="F1:F428"/>
-    <sortCondition ref="G1:G428"/>
-    <sortCondition ref="H1:H428"/>
+  <autoFilter ref="A1:J435" xr:uid="{107DD696-A5A6-CB45-B2DD-8D2A6C9062E3}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:J389">
+    <sortCondition ref="A1:A389"/>
+    <sortCondition ref="B1:B389"/>
+    <sortCondition ref="C1:C389"/>
+    <sortCondition ref="D1:D389"/>
+    <sortCondition ref="E1:E389"/>
+    <sortCondition ref="F1:F389"/>
+    <sortCondition ref="G1:G389"/>
+    <sortCondition ref="H1:H389"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>